<commit_message>
Improved New Element dialog.
Improved New Element dialog:
The new proejct element wizard no can be directly shown at a given
element crieator wizard. The user this way does not have to select the
category and element.

Still working on data import.
</commit_message>
<xml_diff>
--- a/Data/APC_DATA/Triangle_BI_INCURRED.xlsx
+++ b/Data/APC_DATA/Triangle_BI_INCURRED.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>schadejaar</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
 </sst>
 </file>
@@ -1263,11 +1260,11 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2">
-        <f t="shared" si="2"/>
+        <f>YEAR(C42)-1985</f>
         <v>14</v>
       </c>
       <c r="B42">
-        <f t="shared" si="3"/>
+        <f>YEAR(D42)-YEAR(C42)+2</f>
         <v>7</v>
       </c>
       <c r="C42" s="4">
@@ -1287,7 +1284,7 @@
         <v>15</v>
       </c>
       <c r="B43">
-        <f t="shared" si="3"/>
+        <f>YEAR(D43)-YEAR(C43)+2</f>
         <v>2</v>
       </c>
       <c r="C43" s="4">
@@ -1316,8 +1313,9 @@
       <c r="D44" s="4">
         <v>36892</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>14</v>
+      <c r="E44">
+        <f t="shared" ca="1" si="4"/>
+        <v>1205269.5970000017</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1581,7 +1579,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">

</xml_diff>

<commit_message>
Working on data view explorer
</commit_message>
<xml_diff>
--- a/Data/APC_DATA/Triangle_BI_INCURRED.xlsx
+++ b/Data/APC_DATA/Triangle_BI_INCURRED.xlsx
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="dfd">dfd!$A$1:$I$9</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>schadejaar</t>
   </si>
@@ -60,12 +60,18 @@
   <si>
     <t>Value</t>
   </si>
+  <si>
+    <t>First row</t>
+  </si>
+  <si>
+    <t>Data-Type</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -75,6 +81,10 @@
       <name val="MS Sans Serif"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="MS Sans Serif"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,12 +107,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E57" sqref="C22:E57"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -790,7 +801,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:16">
       <c r="A17" s="1">
         <v>2002</v>
       </c>
@@ -811,7 +822,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:16">
       <c r="A18" s="1">
         <v>2003</v>
       </c>
@@ -828,7 +839,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:16">
       <c r="A19" s="1">
         <v>2004</v>
       </c>
@@ -841,746 +852,1293 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:16">
       <c r="A21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="2">
-        <f>YEAR(C22)-1985</f>
+      <c r="G23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B22">
-        <f>YEAR(D22)-YEAR(C22)+2</f>
+      <c r="I23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="2">
+        <f>$B$21</f>
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <f>YEAR(D24)-YEAR(C24)+2</f>
         <v>2</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C24" s="4">
         <v>35431</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D24" s="4">
         <v>35431</v>
       </c>
-      <c r="E22">
-        <f ca="1">INDIRECT(ADDRESS(A22,B22))</f>
+      <c r="E24">
+        <f ca="1">INDIRECT(ADDRESS(A24,B24))</f>
         <v>3013647.7849999988</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="2">
-        <f t="shared" ref="A23:A57" si="2">YEAR(C23)-1985</f>
+      <c r="G24" s="2">
+        <f t="shared" ref="G24:G30" si="2">$B$21</f>
         <v>12</v>
       </c>
-      <c r="B23">
-        <f t="shared" ref="B23:B57" si="3">YEAR(D23)-YEAR(C23)+2</f>
+      <c r="H24">
+        <f t="shared" ref="H24:H51" si="3">YEAR(J24)-YEAR(I24)+2</f>
+        <v>2</v>
+      </c>
+      <c r="I24" s="4">
+        <v>35431</v>
+      </c>
+      <c r="J24" s="4">
+        <v>35431</v>
+      </c>
+      <c r="K24">
+        <f t="shared" ref="K24:K51" ca="1" si="4">INDIRECT(ADDRESS(G24,H24))</f>
+        <v>3013647.7849999988</v>
+      </c>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="2">
+        <f t="shared" ref="A25:A31" si="5">$B$21</f>
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:B59" si="6">YEAR(D25)-YEAR(C25)+2</f>
         <v>3</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C25" s="4">
         <v>35431</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D25" s="4">
         <v>35796</v>
       </c>
-      <c r="E23">
-        <f t="shared" ref="E23:E57" ca="1" si="4">INDIRECT(ADDRESS(A23,B23))</f>
+      <c r="E25">
+        <f t="shared" ref="E25:E59" ca="1" si="7">INDIRECT(ADDRESS(A25,B25))</f>
         <v>825877.97700000647</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="2">
+      <c r="G25" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B24">
-        <f t="shared" si="3"/>
+      <c r="H25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I25" s="4">
+        <v>35431</v>
+      </c>
+      <c r="J25" s="4">
+        <v>35796</v>
+      </c>
+      <c r="K25">
+        <f t="shared" ca="1" si="4"/>
+        <v>825877.97700000647</v>
+      </c>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="2">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C26" s="4">
         <v>35431</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D26" s="4">
         <v>36161</v>
       </c>
-      <c r="E24">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E26">
+        <f t="shared" ca="1" si="7"/>
         <v>102279.32999999868</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="2">
+      <c r="G26" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B25">
-        <f t="shared" si="3"/>
+      <c r="H26">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I26" s="4">
+        <v>35431</v>
+      </c>
+      <c r="J26" s="4">
+        <v>36161</v>
+      </c>
+      <c r="K26">
+        <f t="shared" ca="1" si="4"/>
+        <v>102279.32999999868</v>
+      </c>
+      <c r="O26" s="5"/>
+      <c r="P26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="2">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C27" s="4">
         <v>35431</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D27" s="4">
         <v>36526</v>
       </c>
-      <c r="E25">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E27">
+        <f t="shared" ca="1" si="7"/>
         <v>1319.6359999980778</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="2">
+      <c r="G27" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B26">
-        <f t="shared" si="3"/>
+      <c r="H27">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I27" s="4">
+        <v>35431</v>
+      </c>
+      <c r="J27" s="4">
+        <v>36526</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ca="1" si="4"/>
+        <v>1319.6359999980778</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="2">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C28" s="4">
         <v>35431</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D28" s="4">
         <v>36892</v>
       </c>
-      <c r="E26">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E28">
+        <f t="shared" ca="1" si="7"/>
         <v>8629.7400000006892</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="2">
+      <c r="G28" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="3"/>
+      <c r="H28">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="I28" s="4">
+        <v>35431</v>
+      </c>
+      <c r="J28" s="4">
+        <v>36892</v>
+      </c>
+      <c r="K28">
+        <f t="shared" ca="1" si="4"/>
+        <v>8629.7400000006892</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="2">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C29" s="4">
         <v>35431</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D29" s="4">
         <v>37257</v>
       </c>
-      <c r="E27">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E29">
+        <f t="shared" ca="1" si="7"/>
         <v>284435.07799999649</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="2">
+      <c r="G29" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B28">
-        <f t="shared" si="3"/>
+      <c r="H29">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="I29" s="4">
+        <v>35431</v>
+      </c>
+      <c r="J29" s="4">
+        <v>37257</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ca="1" si="4"/>
+        <v>284435.07799999649</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="2">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C30" s="4">
         <v>35431</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D30" s="4">
         <v>37622</v>
       </c>
-      <c r="E28">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E30">
+        <f t="shared" ca="1" si="7"/>
         <v>-127450.51099999715</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="2">
+      <c r="G30" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B29">
-        <f t="shared" si="3"/>
+      <c r="H30">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I30" s="4">
+        <v>35431</v>
+      </c>
+      <c r="J30" s="4">
+        <v>37622</v>
+      </c>
+      <c r="K30">
+        <f t="shared" ca="1" si="4"/>
+        <v>-127450.51099999715</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="2">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C31" s="4">
         <v>35431</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D31" s="4">
         <v>37987</v>
       </c>
-      <c r="E29">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E31">
+        <f t="shared" ca="1" si="7"/>
         <v>-119869.49500000011</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="2">
-        <f t="shared" si="2"/>
+      <c r="G31" s="2">
+        <f t="shared" ref="G31:G36" si="8">$B$21+1</f>
         <v>13</v>
       </c>
-      <c r="B30">
+      <c r="H31">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="C30" s="4">
+      <c r="I31" s="4">
         <v>35796</v>
       </c>
-      <c r="D30" s="4">
+      <c r="J31" s="4">
         <v>35796</v>
       </c>
-      <c r="E30">
+      <c r="K31">
         <f t="shared" ca="1" si="4"/>
         <v>1677038.9019999984</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="2">
-        <f t="shared" si="2"/>
+    <row r="32" spans="1:16">
+      <c r="A32" s="2">
+        <f>$B$21+1</f>
         <v>13</v>
       </c>
-      <c r="B31">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="C31" s="4">
-        <v>35796</v>
-      </c>
-      <c r="D31" s="4">
-        <v>36161</v>
-      </c>
-      <c r="E31">
-        <f t="shared" ca="1" si="4"/>
-        <v>239628.50200000079</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="2">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
       <c r="B32">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>2</v>
       </c>
       <c r="C32" s="4">
         <v>35796</v>
       </c>
       <c r="D32" s="4">
-        <v>36526</v>
+        <v>35796</v>
       </c>
       <c r="E32">
-        <f t="shared" ca="1" si="4"/>
-        <v>114674.8330000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <f t="shared" ca="1" si="7"/>
+        <v>1677038.9019999984</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I32" s="4">
+        <v>35796</v>
+      </c>
+      <c r="J32" s="4">
+        <v>36161</v>
+      </c>
+      <c r="K32">
+        <f t="shared" ca="1" si="4"/>
+        <v>239628.50200000079</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A33:A38" si="9">$B$21+1</f>
         <v>13</v>
       </c>
       <c r="B33">
-        <f t="shared" si="3"/>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="C33" s="4">
         <v>35796</v>
       </c>
       <c r="D33" s="4">
-        <v>36892</v>
+        <v>36161</v>
       </c>
       <c r="E33">
-        <f t="shared" ca="1" si="4"/>
-        <v>280201.9570000004</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <f t="shared" ca="1" si="7"/>
+        <v>239628.50200000079</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I33" s="4">
+        <v>35796</v>
+      </c>
+      <c r="J33" s="4">
+        <v>36526</v>
+      </c>
+      <c r="K33">
+        <f t="shared" ca="1" si="4"/>
+        <v>114674.8330000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="B34">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="C34" s="4">
         <v>35796</v>
       </c>
       <c r="D34" s="4">
-        <v>37257</v>
+        <v>36526</v>
       </c>
       <c r="E34">
-        <f t="shared" ca="1" si="4"/>
-        <v>517838.72599999839</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <f t="shared" ca="1" si="7"/>
+        <v>114674.8330000001</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I34" s="4">
+        <v>35796</v>
+      </c>
+      <c r="J34" s="4">
+        <v>36892</v>
+      </c>
+      <c r="K34">
+        <f t="shared" ca="1" si="4"/>
+        <v>280201.9570000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="B35">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="C35" s="4">
         <v>35796</v>
       </c>
       <c r="D35" s="4">
-        <v>37622</v>
+        <v>36892</v>
       </c>
       <c r="E35">
-        <f t="shared" ca="1" si="4"/>
-        <v>-114008.66200000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <f t="shared" ca="1" si="7"/>
+        <v>280201.9570000004</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="I35" s="4">
+        <v>35796</v>
+      </c>
+      <c r="J35" s="4">
+        <v>37257</v>
+      </c>
+      <c r="K35">
+        <f t="shared" ca="1" si="4"/>
+        <v>517838.72599999839</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="B36">
-        <f t="shared" si="3"/>
-        <v>8</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="C36" s="4">
         <v>35796</v>
       </c>
       <c r="D36" s="4">
+        <v>37257</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ca="1" si="7"/>
+        <v>517838.72599999839</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="I36" s="4">
+        <v>35796</v>
+      </c>
+      <c r="J36" s="4">
+        <v>37622</v>
+      </c>
+      <c r="K36">
+        <f t="shared" ca="1" si="4"/>
+        <v>-114008.66200000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="2">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C37" s="4">
+        <v>35796</v>
+      </c>
+      <c r="D37" s="4">
+        <v>37622</v>
+      </c>
+      <c r="E37">
+        <f t="shared" ca="1" si="7"/>
+        <v>-114008.66200000001</v>
+      </c>
+      <c r="G37" s="2">
+        <f>$B$21+2</f>
+        <v>14</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I37" s="4">
+        <v>36161</v>
+      </c>
+      <c r="J37" s="4">
+        <v>36161</v>
+      </c>
+      <c r="K37">
+        <f t="shared" ca="1" si="4"/>
+        <v>2119736.7370000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="2">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="C38" s="4">
+        <v>35796</v>
+      </c>
+      <c r="D38" s="4">
         <v>37987</v>
       </c>
-      <c r="E36">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E38">
+        <f t="shared" ca="1" si="7"/>
         <v>-208186.88100000052</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2">
-        <f t="shared" si="2"/>
+      <c r="G38" s="2">
+        <f>$B$21+2</f>
         <v>14</v>
       </c>
-      <c r="B37">
-        <f t="shared" si="3"/>
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I38" s="4">
+        <v>36161</v>
+      </c>
+      <c r="J38" s="4">
+        <v>36526</v>
+      </c>
+      <c r="K38">
+        <f t="shared" ca="1" si="4"/>
+        <v>365194.39599999972</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="2">
+        <f t="shared" ref="A39:A44" si="10">$B$21+2</f>
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="6"/>
         <v>2</v>
-      </c>
-      <c r="C37" s="4">
-        <v>36161</v>
-      </c>
-      <c r="D37" s="4">
-        <v>36161</v>
-      </c>
-      <c r="E37">
-        <f t="shared" ca="1" si="4"/>
-        <v>2119736.7370000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="C38" s="4">
-        <v>36161</v>
-      </c>
-      <c r="D38" s="4">
-        <v>36526</v>
-      </c>
-      <c r="E38">
-        <f t="shared" ca="1" si="4"/>
-        <v>365194.39599999972</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="2">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="3"/>
-        <v>4</v>
       </c>
       <c r="C39" s="4">
         <v>36161</v>
       </c>
       <c r="D39" s="4">
+        <v>36161</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ca="1" si="7"/>
+        <v>2119736.7370000002</v>
+      </c>
+      <c r="G39" s="2">
+        <f>$B$21+2</f>
+        <v>14</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I39" s="4">
+        <v>36161</v>
+      </c>
+      <c r="J39" s="4">
         <v>36892</v>
       </c>
-      <c r="E39">
+      <c r="K39">
         <f t="shared" ca="1" si="4"/>
         <v>240915.16800000332</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:11">
       <c r="A40" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="B40">
-        <f t="shared" si="3"/>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="C40" s="4">
         <v>36161</v>
       </c>
       <c r="D40" s="4">
+        <v>36526</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ca="1" si="7"/>
+        <v>365194.39599999972</v>
+      </c>
+      <c r="G40" s="2">
+        <f>$B$21+2</f>
+        <v>14</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I40" s="4">
+        <v>36161</v>
+      </c>
+      <c r="J40" s="4">
         <v>37257</v>
       </c>
-      <c r="E40">
+      <c r="K40">
         <f t="shared" ca="1" si="4"/>
         <v>603489.25799999852</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:11">
       <c r="A41" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="B41">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="C41" s="4">
         <v>36161</v>
       </c>
       <c r="D41" s="4">
+        <v>36892</v>
+      </c>
+      <c r="E41">
+        <f t="shared" ca="1" si="7"/>
+        <v>240915.16800000332</v>
+      </c>
+      <c r="G41" s="2">
+        <f>$B$21+2</f>
+        <v>14</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="I41" s="4">
+        <v>36161</v>
+      </c>
+      <c r="J41" s="4">
         <v>37622</v>
       </c>
-      <c r="E41">
+      <c r="K41">
         <f t="shared" ca="1" si="4"/>
         <v>1837.5260000005364</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:11">
       <c r="A42" s="2">
-        <f>YEAR(C42)-1985</f>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="B42">
-        <f>YEAR(D42)-YEAR(C42)+2</f>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="C42" s="4">
         <v>36161</v>
       </c>
       <c r="D42" s="4">
+        <v>37257</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ca="1" si="7"/>
+        <v>603489.25799999852</v>
+      </c>
+      <c r="G42" s="2">
+        <f>$B$21+3</f>
+        <v>15</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I42" s="4">
+        <v>36526</v>
+      </c>
+      <c r="J42" s="4">
+        <v>36526</v>
+      </c>
+      <c r="K42">
+        <f t="shared" ca="1" si="4"/>
+        <v>1947059.996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="2">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="C43" s="4">
+        <v>36161</v>
+      </c>
+      <c r="D43" s="4">
+        <v>37622</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ca="1" si="7"/>
+        <v>1837.5260000005364</v>
+      </c>
+      <c r="G43" s="2">
+        <f>$B$21+3</f>
+        <v>15</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I43" s="4">
+        <v>36526</v>
+      </c>
+      <c r="J43" s="4">
+        <v>36892</v>
+      </c>
+      <c r="K43">
+        <f t="shared" ca="1" si="4"/>
+        <v>1205269.5970000017</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="2">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <f>YEAR(D44)-YEAR(C44)+2</f>
+        <v>7</v>
+      </c>
+      <c r="C44" s="4">
+        <v>36161</v>
+      </c>
+      <c r="D44" s="4">
         <v>37987</v>
       </c>
-      <c r="E42">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E44">
+        <f t="shared" ca="1" si="7"/>
         <v>-273750.98600000003</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="2">
-        <f t="shared" si="2"/>
+      <c r="G44" s="2">
+        <f>$B$21+3</f>
         <v>15</v>
       </c>
-      <c r="B43">
-        <f>YEAR(D43)-YEAR(C43)+2</f>
+      <c r="H44">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I44" s="4">
+        <v>36526</v>
+      </c>
+      <c r="J44" s="4">
+        <v>37257</v>
+      </c>
+      <c r="K44">
+        <f t="shared" ca="1" si="4"/>
+        <v>774418.24599999888</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="2">
+        <f>$B$21+3</f>
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <f>YEAR(D45)-YEAR(C45)+2</f>
         <v>2</v>
-      </c>
-      <c r="C43" s="4">
-        <v>36526</v>
-      </c>
-      <c r="D43" s="4">
-        <v>36526</v>
-      </c>
-      <c r="E43">
-        <f t="shared" ca="1" si="4"/>
-        <v>1947059.996</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="2">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="B44">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="C44" s="4">
-        <v>36526</v>
-      </c>
-      <c r="D44" s="4">
-        <v>36892</v>
-      </c>
-      <c r="E44">
-        <f t="shared" ca="1" si="4"/>
-        <v>1205269.5970000017</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="2">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="B45">
-        <f t="shared" si="3"/>
-        <v>4</v>
       </c>
       <c r="C45" s="4">
         <v>36526</v>
       </c>
       <c r="D45" s="4">
-        <v>37257</v>
+        <v>36526</v>
       </c>
       <c r="E45">
-        <f t="shared" ca="1" si="4"/>
-        <v>774418.24599999888</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <f t="shared" ca="1" si="7"/>
+        <v>1947059.996</v>
+      </c>
+      <c r="G45" s="2">
+        <f>$B$21+3</f>
+        <v>15</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I45" s="4">
+        <v>36526</v>
+      </c>
+      <c r="J45" s="4">
+        <v>37622</v>
+      </c>
+      <c r="K45">
+        <f t="shared" ca="1" si="4"/>
+        <v>39256.062999999616</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="2">
-        <f t="shared" si="2"/>
+        <f>$B$21+3</f>
         <v>15</v>
       </c>
       <c r="B46">
-        <f t="shared" si="3"/>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="C46" s="4">
         <v>36526</v>
       </c>
       <c r="D46" s="4">
-        <v>37622</v>
+        <v>36892</v>
       </c>
       <c r="E46">
-        <f t="shared" ca="1" si="4"/>
-        <v>39256.062999999616</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <f t="shared" ca="1" si="7"/>
+        <v>1205269.5970000017</v>
+      </c>
+      <c r="G46" s="2">
+        <f>$B$21+4</f>
+        <v>16</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I46" s="4">
+        <v>36892</v>
+      </c>
+      <c r="J46" s="4">
+        <v>36892</v>
+      </c>
+      <c r="K46">
+        <f t="shared" ca="1" si="4"/>
+        <v>3059368.5990000004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="2">
-        <f t="shared" si="2"/>
+        <f>$B$21+3</f>
         <v>15</v>
       </c>
       <c r="B47">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="C47" s="4">
         <v>36526</v>
       </c>
       <c r="D47" s="4">
+        <v>37257</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ca="1" si="7"/>
+        <v>774418.24599999888</v>
+      </c>
+      <c r="G47" s="2">
+        <f>$B$21+4</f>
+        <v>16</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I47" s="4">
+        <v>36892</v>
+      </c>
+      <c r="J47" s="4">
+        <v>37257</v>
+      </c>
+      <c r="K47">
+        <f t="shared" ca="1" si="4"/>
+        <v>1160423.9729999946</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="2">
+        <f>$B$21+3</f>
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="C48" s="4">
+        <v>36526</v>
+      </c>
+      <c r="D48" s="4">
+        <v>37622</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ca="1" si="7"/>
+        <v>39256.062999999616</v>
+      </c>
+      <c r="G48" s="2">
+        <f>$B$21+4</f>
+        <v>16</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I48" s="4">
+        <v>36892</v>
+      </c>
+      <c r="J48" s="4">
+        <v>37622</v>
+      </c>
+      <c r="K48">
+        <f t="shared" ca="1" si="4"/>
+        <v>526466.42600000184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="2">
+        <f>$B$21+3</f>
+        <v>15</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="C49" s="4">
+        <v>36526</v>
+      </c>
+      <c r="D49" s="4">
         <v>37987</v>
       </c>
-      <c r="E47">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E49">
+        <f t="shared" ca="1" si="7"/>
         <v>189945.53599999985</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="2">
-        <f t="shared" si="2"/>
+      <c r="G49" s="2">
+        <f>$B$21+5</f>
+        <v>17</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I49" s="4">
+        <v>37257</v>
+      </c>
+      <c r="J49" s="4">
+        <v>37257</v>
+      </c>
+      <c r="K49">
+        <f t="shared" ca="1" si="4"/>
+        <v>4320019.1560000107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="2">
+        <f>$B$21+4</f>
         <v>16</v>
       </c>
-      <c r="B48">
-        <f t="shared" si="3"/>
+      <c r="B50">
+        <f t="shared" si="6"/>
         <v>2</v>
-      </c>
-      <c r="C48" s="4">
-        <v>36892</v>
-      </c>
-      <c r="D48" s="4">
-        <v>36892</v>
-      </c>
-      <c r="E48">
-        <f t="shared" ca="1" si="4"/>
-        <v>3059368.5990000004</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="2">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="B49">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="C49" s="4">
-        <v>36892</v>
-      </c>
-      <c r="D49" s="4">
-        <v>37257</v>
-      </c>
-      <c r="E49">
-        <f t="shared" ca="1" si="4"/>
-        <v>1160423.9729999946</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="2">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="B50">
-        <f t="shared" si="3"/>
-        <v>4</v>
       </c>
       <c r="C50" s="4">
         <v>36892</v>
       </c>
       <c r="D50" s="4">
+        <v>36892</v>
+      </c>
+      <c r="E50">
+        <f t="shared" ca="1" si="7"/>
+        <v>3059368.5990000004</v>
+      </c>
+      <c r="G50" s="2">
+        <f>$B$21+5</f>
+        <v>17</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I50" s="4">
+        <v>37257</v>
+      </c>
+      <c r="J50" s="4">
         <v>37622</v>
       </c>
-      <c r="E50">
-        <f t="shared" ca="1" si="4"/>
-        <v>526466.42600000184</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="K50">
+        <f t="shared" ca="1" si="4"/>
+        <v>-105700.75000000931</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="2">
-        <f t="shared" si="2"/>
+        <f>$B$21+4</f>
         <v>16</v>
       </c>
       <c r="B51">
-        <f t="shared" si="3"/>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="C51" s="4">
         <v>36892</v>
       </c>
       <c r="D51" s="4">
+        <v>37257</v>
+      </c>
+      <c r="E51">
+        <f t="shared" ca="1" si="7"/>
+        <v>1160423.9729999946</v>
+      </c>
+      <c r="G51" s="2">
+        <f>$B$21+6</f>
+        <v>18</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I51" s="4">
+        <v>37622</v>
+      </c>
+      <c r="J51" s="4">
+        <v>37622</v>
+      </c>
+      <c r="K51">
+        <f t="shared" ca="1" si="4"/>
+        <v>2713203.4650000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="2">
+        <f>$B$21+4</f>
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="C52" s="4">
+        <v>36892</v>
+      </c>
+      <c r="D52" s="4">
+        <v>37622</v>
+      </c>
+      <c r="E52">
+        <f t="shared" ca="1" si="7"/>
+        <v>526466.42600000184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="2">
+        <f>$B$21+4</f>
+        <v>16</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="C53" s="4">
+        <v>36892</v>
+      </c>
+      <c r="D53" s="4">
         <v>37987</v>
       </c>
-      <c r="E51">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E53">
+        <f t="shared" ca="1" si="7"/>
         <v>352815.52699999698</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="2">
-        <f t="shared" si="2"/>
+      <c r="G53" s="2"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="2">
+        <f>$B$21+5</f>
         <v>17</v>
       </c>
-      <c r="B52">
-        <f t="shared" si="3"/>
+      <c r="B54">
+        <f t="shared" si="6"/>
         <v>2</v>
-      </c>
-      <c r="C52" s="4">
-        <v>37257</v>
-      </c>
-      <c r="D52" s="4">
-        <v>37257</v>
-      </c>
-      <c r="E52">
-        <f t="shared" ca="1" si="4"/>
-        <v>4320019.1560000107</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="2">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="B53">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="C53" s="4">
-        <v>37257</v>
-      </c>
-      <c r="D53" s="4">
-        <v>37622</v>
-      </c>
-      <c r="E53">
-        <f t="shared" ca="1" si="4"/>
-        <v>-105700.75000000931</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="2">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="B54">
-        <f t="shared" si="3"/>
-        <v>4</v>
       </c>
       <c r="C54" s="4">
         <v>37257</v>
       </c>
       <c r="D54" s="4">
-        <v>37987</v>
+        <v>37257</v>
       </c>
       <c r="E54">
-        <f t="shared" ca="1" si="4"/>
-        <v>1211410.1469999989</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <f t="shared" ca="1" si="7"/>
+        <v>4320019.1560000107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="2">
-        <f t="shared" si="2"/>
-        <v>18</v>
+        <f>$B$21+5</f>
+        <v>17</v>
       </c>
       <c r="B55">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="C55" s="4">
-        <v>37622</v>
+        <v>37257</v>
       </c>
       <c r="D55" s="4">
         <v>37622</v>
       </c>
       <c r="E55">
-        <f t="shared" ca="1" si="4"/>
-        <v>2713203.4650000003</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <f t="shared" ca="1" si="7"/>
+        <v>-105700.75000000931</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="2">
-        <f t="shared" si="2"/>
-        <v>18</v>
+        <f>$B$21+5</f>
+        <v>17</v>
       </c>
       <c r="B56">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="C56" s="4">
-        <v>37622</v>
+        <v>37257</v>
       </c>
       <c r="D56" s="4">
         <v>37987</v>
       </c>
       <c r="E56">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="7"/>
+        <v>1211410.1469999989</v>
+      </c>
+      <c r="G56" s="2"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="2">
+        <f>$B$21+6</f>
+        <v>18</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="C57" s="4">
+        <v>37622</v>
+      </c>
+      <c r="D57" s="4">
+        <v>37622</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ca="1" si="7"/>
+        <v>2713203.4650000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="2">
+        <f>$B$21+6</f>
+        <v>18</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="C58" s="4">
+        <v>37622</v>
+      </c>
+      <c r="D58" s="4">
+        <v>37987</v>
+      </c>
+      <c r="E58">
+        <f t="shared" ca="1" si="7"/>
         <v>1083041.5189999994</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="2">
-        <f t="shared" si="2"/>
+      <c r="G58" s="2"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="2">
+        <f>$B$21+7</f>
         <v>19</v>
       </c>
-      <c r="B57">
-        <f t="shared" si="3"/>
+      <c r="B59">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C59" s="4">
         <v>37987</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D59" s="4">
         <v>37987</v>
       </c>
-      <c r="E57">
-        <f t="shared" ca="1" si="4"/>
+      <c r="E59">
+        <f t="shared" ca="1" si="7"/>
         <v>3461298.1089999992</v>
       </c>
+      <c r="G59" s="2"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;A</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>

</xml_diff>